<commit_message>
Profile Page checks added
</commit_message>
<xml_diff>
--- a/DSSTestAutomationFramework1.2/EmailIDTestData.xlsx
+++ b/DSSTestAutomationFramework1.2/EmailIDTestData.xlsx
@@ -4,17 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14460" windowHeight="5535" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="4365" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AOL" sheetId="7" r:id="rId1"/>
-    <sheet name="Twitter" sheetId="6" r:id="rId2"/>
-    <sheet name="Yahoo" sheetId="5" r:id="rId3"/>
-    <sheet name="Gmail" sheetId="3" r:id="rId4"/>
-    <sheet name="Facebook" sheetId="4" r:id="rId5"/>
+    <sheet name="Yahoo" sheetId="5" r:id="rId2"/>
+    <sheet name="Gmail" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M16"/>
+  <oleSize ref="A1:K12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Password</t>
   </si>
@@ -32,9 +30,6 @@
     <t>EmailId</t>
   </si>
   <si>
-    <t>aa@gmail.com</t>
-  </si>
-  <si>
     <t>Tribune1</t>
   </si>
   <si>
@@ -53,25 +48,61 @@
     <t>Tribune6</t>
   </si>
   <si>
-    <t>aa@twitter.com</t>
-  </si>
-  <si>
-    <t>aa@aol.com</t>
-  </si>
-  <si>
-    <t>aa@yahoo.com</t>
-  </si>
-  <si>
-    <t>aa@facbook.com</t>
-  </si>
-  <si>
     <t>tribune1</t>
   </si>
   <si>
-    <t>tribunedss@gmail.com</t>
-  </si>
-  <si>
-    <t>jamesmillerfacbook@gmail.com</t>
+    <t>aa1@aol.com</t>
+  </si>
+  <si>
+    <t>aa2@aol.com</t>
+  </si>
+  <si>
+    <t>aa3@aol.com</t>
+  </si>
+  <si>
+    <t>aa4@aol.com</t>
+  </si>
+  <si>
+    <t>aa5@aol.com</t>
+  </si>
+  <si>
+    <t>aa6@aol.com</t>
+  </si>
+  <si>
+    <t>aa1@yahoo.com</t>
+  </si>
+  <si>
+    <t>aa2@gmail.com</t>
+  </si>
+  <si>
+    <t>aa1@gmail.com</t>
+  </si>
+  <si>
+    <t>aa3@gmail.com</t>
+  </si>
+  <si>
+    <t>aa4@gmail.com</t>
+  </si>
+  <si>
+    <t>aa5@gmail.com</t>
+  </si>
+  <si>
+    <t>aa6@gmail.com</t>
+  </si>
+  <si>
+    <t>aa2@yahoo.com</t>
+  </si>
+  <si>
+    <t>aa3@yahoo.com</t>
+  </si>
+  <si>
+    <t>aa4@yahoo.com</t>
+  </si>
+  <si>
+    <t>aa5@yahoo.com</t>
+  </si>
+  <si>
+    <t>aa6@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -428,7 +459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -445,50 +478,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -496,6 +529,10 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3:A7" r:id="rId2" display="aa@gmail.com"/>
     <hyperlink ref="A7" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="A4" r:id="rId6"/>
+    <hyperlink ref="A3" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -506,7 +543,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,50 +561,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -575,6 +612,10 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3:A7" r:id="rId2" display="aa@gmail.com"/>
     <hyperlink ref="A7" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="A4" r:id="rId6"/>
+    <hyperlink ref="A3" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -584,87 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3:A7" r:id="rId2" display="aa@gmail.com"/>
-    <hyperlink ref="A7" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,50 +644,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -733,85 +695,9 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A7" r:id="rId2"/>
     <hyperlink ref="A6" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3:A7" r:id="rId2" display="aa@gmail.com"/>
-    <hyperlink ref="A7" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="A3" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
internal demo - 2 test cases only
</commit_message>
<xml_diff>
--- a/DSSTestAutomationFramework1.2/EmailIDTestData.xlsx
+++ b/DSSTestAutomationFramework1.2/EmailIDTestData.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="4365" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="4650"/>
   </bookViews>
   <sheets>
-    <sheet name="AOL" sheetId="7" r:id="rId1"/>
-    <sheet name="Yahoo" sheetId="5" r:id="rId2"/>
-    <sheet name="Gmail" sheetId="3" r:id="rId3"/>
+    <sheet name="AOL" sheetId="11" r:id="rId1"/>
+    <sheet name="Yahoo" sheetId="10" r:id="rId2"/>
+    <sheet name="Gmail" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K12"/>
+  <oleSize ref="A1:N13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Password</t>
   </si>
@@ -30,79 +30,49 @@
     <t>EmailId</t>
   </si>
   <si>
-    <t>Tribune1</t>
-  </si>
-  <si>
-    <t>Tribune2</t>
-  </si>
-  <si>
-    <t>Tribune3</t>
-  </si>
-  <si>
-    <t>Tribune4</t>
-  </si>
-  <si>
-    <t>Tribune5</t>
-  </si>
-  <si>
-    <t>Tribune6</t>
-  </si>
-  <si>
     <t>tribune1</t>
   </si>
   <si>
-    <t>aa1@aol.com</t>
-  </si>
-  <si>
-    <t>aa2@aol.com</t>
-  </si>
-  <si>
-    <t>aa3@aol.com</t>
-  </si>
-  <si>
-    <t>aa4@aol.com</t>
-  </si>
-  <si>
-    <t>aa5@aol.com</t>
-  </si>
-  <si>
-    <t>aa6@aol.com</t>
-  </si>
-  <si>
-    <t>aa1@yahoo.com</t>
-  </si>
-  <si>
-    <t>aa2@gmail.com</t>
-  </si>
-  <si>
-    <t>aa1@gmail.com</t>
-  </si>
-  <si>
-    <t>aa3@gmail.com</t>
-  </si>
-  <si>
-    <t>aa4@gmail.com</t>
-  </si>
-  <si>
-    <t>aa5@gmail.com</t>
-  </si>
-  <si>
-    <t>aa6@gmail.com</t>
-  </si>
-  <si>
-    <t>aa2@yahoo.com</t>
-  </si>
-  <si>
-    <t>aa3@yahoo.com</t>
-  </si>
-  <si>
-    <t>aa4@yahoo.com</t>
-  </si>
-  <si>
-    <t>aa5@yahoo.com</t>
-  </si>
-  <si>
-    <t>aa6@yahoo.com</t>
+    <t>jamesmillermay12@aol.com</t>
+  </si>
+  <si>
+    <t>ssortest1100@aol.com</t>
+  </si>
+  <si>
+    <t>ssortest3344@aol.com</t>
+  </si>
+  <si>
+    <t>ssortest21@yahoo.com</t>
+  </si>
+  <si>
+    <t>ssortest22@yahoo.com</t>
+  </si>
+  <si>
+    <t>ssortest24@yahoo.com</t>
+  </si>
+  <si>
+    <t>ssortest25@yahoo.com</t>
+  </si>
+  <si>
+    <t>ssortest26@yahoo.com</t>
+  </si>
+  <si>
+    <t>ssortest21@gmail.com</t>
+  </si>
+  <si>
+    <t>ssortest22@gmail.com</t>
+  </si>
+  <si>
+    <t>ssortest23@gmail.com</t>
+  </si>
+  <si>
+    <t>ssortest24@gmail.com</t>
+  </si>
+  <si>
+    <t>ssortest25@gmail.com</t>
+  </si>
+  <si>
+    <t>tribune2</t>
   </si>
 </sst>
 </file>
@@ -173,8 +143,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -457,16 +427,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -478,7 +445,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -486,53 +453,25 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3:A7" r:id="rId2" display="aa@gmail.com"/>
-    <hyperlink ref="A7" r:id="rId3"/>
-    <hyperlink ref="A6" r:id="rId4"/>
-    <hyperlink ref="A5" r:id="rId5"/>
-    <hyperlink ref="A4" r:id="rId6"/>
-    <hyperlink ref="A3" r:id="rId7"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -540,16 +479,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -561,61 +497,52 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
+      <c r="A3" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
+      <c r="A4" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
+      <c r="A5" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
+      <c r="A6" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3:A7" r:id="rId2" display="aa@gmail.com"/>
-    <hyperlink ref="A7" r:id="rId3"/>
-    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4:A6" r:id="rId3" display="mailto:ssortest21@yahoo.com"/>
+    <hyperlink ref="A4" r:id="rId4"/>
     <hyperlink ref="A5" r:id="rId5"/>
-    <hyperlink ref="A4" r:id="rId6"/>
-    <hyperlink ref="A3" r:id="rId7"/>
+    <hyperlink ref="A6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -623,16 +550,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -644,7 +568,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -652,52 +576,44 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A7" r:id="rId2"/>
-    <hyperlink ref="A6" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
-    <hyperlink ref="A3" r:id="rId6"/>
+    <hyperlink ref="A3:A6" r:id="rId2" display="ssortest21@gmail.com "/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="A6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
internal demo -  2 test cases
</commit_message>
<xml_diff>
--- a/DSSTestAutomationFramework1.2/EmailIDTestData.xlsx
+++ b/DSSTestAutomationFramework1.2/EmailIDTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="4365" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AOL" sheetId="11" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Gmail" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N13"/>
+  <oleSize ref="A4:N15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -429,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -552,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>